<commit_message>
Update dataset for analysis and simulation experiments
</commit_message>
<xml_diff>
--- a/data set.xlsx
+++ b/data set.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="156">
   <si>
     <t>Event id</t>
   </si>
@@ -60,7 +60,7 @@
     <t xml:space="preserve">7.40 a.m </t>
   </si>
   <si>
-    <t xml:space="preserve">7.30 a.m. </t>
+    <t xml:space="preserve">8.30 a.m. </t>
   </si>
   <si>
     <t>E002</t>
@@ -72,7 +72,7 @@
     <t>8.00 a.m</t>
   </si>
   <si>
-    <t xml:space="preserve">7.55 a.m. </t>
+    <t xml:space="preserve">8.55 a.m. </t>
   </si>
   <si>
     <t>E003</t>
@@ -81,127 +81,133 @@
     <t>F003</t>
   </si>
   <si>
+    <t>8.40 a.m</t>
+  </si>
+  <si>
+    <t>E004</t>
+  </si>
+  <si>
+    <t>F004</t>
+  </si>
+  <si>
+    <t>9.50 a.m</t>
+  </si>
+  <si>
+    <t>E005</t>
+  </si>
+  <si>
+    <t>F005</t>
+  </si>
+  <si>
+    <t>8.50 a.m</t>
+  </si>
+  <si>
+    <t>9.30 a.m</t>
+  </si>
+  <si>
+    <t>E006</t>
+  </si>
+  <si>
+    <t>F006</t>
+  </si>
+  <si>
+    <t>Day 02</t>
+  </si>
+  <si>
+    <t>8.10 a.m</t>
+  </si>
+  <si>
+    <t>9.15 a.m</t>
+  </si>
+  <si>
+    <t>E007</t>
+  </si>
+  <si>
+    <t>F007</t>
+  </si>
+  <si>
+    <t>8.25 a.m</t>
+  </si>
+  <si>
+    <t>E008</t>
+  </si>
+  <si>
+    <t>F008</t>
+  </si>
+  <si>
+    <t>8.30 a.m</t>
+  </si>
+  <si>
+    <t>9.25 a.m</t>
+  </si>
+  <si>
+    <t>Avg wait (min)</t>
+  </si>
+  <si>
+    <t>Avg queue length (Per dock)</t>
+  </si>
+  <si>
+    <t>E009</t>
+  </si>
+  <si>
+    <t>F009</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>E010</t>
+  </si>
+  <si>
+    <t>F010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45 a.m </t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>E011</t>
+  </si>
+  <si>
+    <t>F011</t>
+  </si>
+  <si>
+    <t>Day 03</t>
+  </si>
+  <si>
+    <t>7.15 a.m</t>
+  </si>
+  <si>
+    <t>7.55 a.m</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>E012</t>
+  </si>
+  <si>
+    <t>F012</t>
+  </si>
+  <si>
+    <t>7.35 a.m</t>
+  </si>
+  <si>
+    <t>Day 4</t>
+  </si>
+  <si>
+    <t>E013</t>
+  </si>
+  <si>
+    <t>F013</t>
+  </si>
+  <si>
     <t>7.40 a.m</t>
   </si>
   <si>
-    <t>E004</t>
-  </si>
-  <si>
-    <t>F004</t>
-  </si>
-  <si>
-    <t>8.40 a.m</t>
-  </si>
-  <si>
-    <t>8.50 a.m</t>
-  </si>
-  <si>
-    <t>E005</t>
-  </si>
-  <si>
-    <t>F005</t>
-  </si>
-  <si>
-    <t>8.30 a.m</t>
-  </si>
-  <si>
-    <t>E006</t>
-  </si>
-  <si>
-    <t>F006</t>
-  </si>
-  <si>
-    <t>Day 02</t>
-  </si>
-  <si>
-    <t>8.10 a.m</t>
-  </si>
-  <si>
-    <t>8.15 a.m</t>
-  </si>
-  <si>
-    <t>E007</t>
-  </si>
-  <si>
-    <t>F007</t>
-  </si>
-  <si>
-    <t>8.25 a.m</t>
-  </si>
-  <si>
-    <t>E008</t>
-  </si>
-  <si>
-    <t>F008</t>
-  </si>
-  <si>
-    <t>Avg wait (min)</t>
-  </si>
-  <si>
-    <t>Avg queue length (Per dock)</t>
-  </si>
-  <si>
-    <t>E009</t>
-  </si>
-  <si>
-    <t>F009</t>
-  </si>
-  <si>
-    <t>Day 1</t>
-  </si>
-  <si>
-    <t>E010</t>
-  </si>
-  <si>
-    <t>F010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.45 a.m </t>
-  </si>
-  <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>E011</t>
-  </si>
-  <si>
-    <t>F011</t>
-  </si>
-  <si>
-    <t>Day 03</t>
-  </si>
-  <si>
-    <t>7.15 a.m</t>
-  </si>
-  <si>
-    <t>6.55 a.m</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>E012</t>
-  </si>
-  <si>
-    <t>F012</t>
-  </si>
-  <si>
-    <t>7.35 a.m</t>
-  </si>
-  <si>
-    <t>7.25 a.m</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>E013</t>
-  </si>
-  <si>
-    <t>F013</t>
-  </si>
-  <si>
-    <t>7.55 a.m</t>
+    <t>8.55 a.m</t>
   </si>
   <si>
     <t>E014</t>
@@ -213,7 +219,7 @@
     <t>7.45 a.m</t>
   </si>
   <si>
-    <t>8.05 a.m</t>
+    <t>9.05 a.m</t>
   </si>
   <si>
     <t>E015</t>
@@ -225,7 +231,7 @@
     <t xml:space="preserve">7.50 a.m </t>
   </si>
   <si>
-    <t xml:space="preserve">7.35 a.m </t>
+    <t xml:space="preserve">8.35 a.m </t>
   </si>
   <si>
     <t>E016</t>
@@ -237,13 +243,16 @@
     <t>Day 04</t>
   </si>
   <si>
+    <t>9.40 a.m</t>
+  </si>
+  <si>
     <t>E017</t>
   </si>
   <si>
     <t>F017</t>
   </si>
   <si>
-    <t xml:space="preserve">8.35 a.m </t>
+    <t xml:space="preserve">9.35 a.m </t>
   </si>
   <si>
     <t>E018</t>
@@ -252,7 +261,7 @@
     <t>F018</t>
   </si>
   <si>
-    <t>8.20 a.m</t>
+    <t>9.20 a.m</t>
   </si>
   <si>
     <t>E019</t>
@@ -264,7 +273,7 @@
     <t>9.10 a.m</t>
   </si>
   <si>
-    <t>8.55 a.m</t>
+    <t>9.55 a.m</t>
   </si>
   <si>
     <t>E020</t>
@@ -276,7 +285,7 @@
     <t xml:space="preserve">9.15 a.m </t>
   </si>
   <si>
-    <t>9.20 a.m</t>
+    <t>10.20 a.m</t>
   </si>
   <si>
     <t>Dock id</t>
@@ -1011,19 +1020,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
@@ -1031,19 +1040,19 @@
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E2" s="8">
         <v>780</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
@@ -1052,16 +1061,16 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="36" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E3" s="8">
         <v>820</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -1070,16 +1079,16 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="36" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E4" s="8">
         <v>550</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -1088,34 +1097,34 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="36" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E5" s="8">
         <v>910</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="11" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E6" s="14">
         <v>630</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
@@ -1126,16 +1135,16 @@
         <v>31</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>138</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>135</v>
       </c>
       <c r="E7" s="19">
         <v>1200</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
@@ -1144,16 +1153,16 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="36" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E8" s="8">
         <v>1000</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
@@ -1162,236 +1171,236 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="36" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E9" s="8">
         <v>950</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="36" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E10" s="8">
         <v>960</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E11" s="14">
         <v>850</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E12" s="19">
         <v>770</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="36" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E13" s="8">
         <v>900</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="36" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E14" s="8">
         <v>1100</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="36" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E15" s="8">
         <v>1400</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="11" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E16" s="14">
         <v>950</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E17" s="19">
         <v>1350</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="36" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E18" s="8">
         <v>1080</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="36" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E19" s="8">
         <v>870</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="36" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E20" s="8">
         <v>700</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="11" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E21" s="14">
         <v>1200</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1432,15 +1441,15 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
       <c r="A1" s="29" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="31" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
@@ -1453,13 +1462,13 @@
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -1468,10 +1477,10 @@
         <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1480,7 +1489,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -1492,16 +1501,16 @@
         <f> B3+C3</f>
       </c>
       <c r="E3" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1510,7 +1519,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
@@ -1522,16 +1531,16 @@
         <f> B4+C4</f>
       </c>
       <c r="E4" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1540,7 +1549,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
@@ -1552,16 +1561,16 @@
         <f> B5+C5</f>
       </c>
       <c r="E5" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -1570,7 +1579,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B6" s="8">
         <v>1</v>
@@ -1582,27 +1591,27 @@
         <f> B6+C6</f>
       </c>
       <c r="E6" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="33" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="L6" s="34"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B7" s="8">
         <v>1</v>
@@ -1614,16 +1623,16 @@
         <f> B7+C7</f>
       </c>
       <c r="E7" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -1636,7 +1645,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B8" s="8">
         <v>1</v>
@@ -1648,16 +1657,16 @@
         <f> B8+C8</f>
       </c>
       <c r="E8" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1670,7 +1679,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
@@ -1682,21 +1691,21 @@
         <f> B9+C9</f>
       </c>
       <c r="E9" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L9" s="8">
         <v>27</v>
@@ -1704,7 +1713,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
@@ -1716,21 +1725,21 @@
         <f> B10+C10</f>
       </c>
       <c r="E10" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L10" s="14">
         <v>27</v>
@@ -1738,7 +1747,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -1750,16 +1759,16 @@
         <f> B11+C11</f>
       </c>
       <c r="E11" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -1768,7 +1777,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B12" s="8">
         <v>1</v>
@@ -1780,16 +1789,16 @@
         <f> B12+C12</f>
       </c>
       <c r="E12" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1798,7 +1807,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B13" s="8">
         <v>1</v>
@@ -1810,16 +1819,16 @@
         <f> B13+C13</f>
       </c>
       <c r="E13" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1828,7 +1837,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B14" s="8">
         <v>1</v>
@@ -1840,16 +1849,16 @@
         <f> B14+C14</f>
       </c>
       <c r="E14" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1858,7 +1867,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
@@ -1870,16 +1879,16 @@
         <f> B15+C15</f>
       </c>
       <c r="E15" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1888,7 +1897,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B16" s="8">
         <v>2</v>
@@ -1900,16 +1909,16 @@
         <f> B16+C16</f>
       </c>
       <c r="E16" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1918,7 +1927,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B17" s="8">
         <v>1</v>
@@ -1930,16 +1939,16 @@
         <f> B17+C17</f>
       </c>
       <c r="E17" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1948,7 +1957,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B18" s="8">
         <v>2</v>
@@ -1960,16 +1969,16 @@
         <f> B18+C18</f>
       </c>
       <c r="E18" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1978,7 +1987,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B19" s="8">
         <v>1</v>
@@ -1990,16 +1999,16 @@
         <f> B19+C19</f>
       </c>
       <c r="E19" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -2008,7 +2017,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B20" s="8">
         <v>1</v>
@@ -2020,16 +2029,16 @@
         <f> B20+C20</f>
       </c>
       <c r="E20" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -2038,7 +2047,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B21" s="8">
         <v>1</v>
@@ -2050,16 +2059,16 @@
         <f> B21+C21</f>
       </c>
       <c r="E21" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -2068,7 +2077,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B22" s="8">
         <v>2</v>
@@ -2080,16 +2089,16 @@
         <f> B22+C22</f>
       </c>
       <c r="E22" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -2098,7 +2107,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B23" s="8">
         <v>1</v>
@@ -2110,16 +2119,16 @@
         <f> B23+C23</f>
       </c>
       <c r="E23" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -2128,7 +2137,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B24" s="8">
         <v>1</v>
@@ -2140,16 +2149,16 @@
         <f> B24+C24</f>
       </c>
       <c r="E24" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -2158,7 +2167,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B25" s="8">
         <v>1</v>
@@ -2170,16 +2179,16 @@
         <f> B25+C25</f>
       </c>
       <c r="E25" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -2188,7 +2197,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B26" s="8">
         <v>1</v>
@@ -2200,16 +2209,16 @@
         <f> B26+C26</f>
       </c>
       <c r="E26" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -2218,7 +2227,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B27" s="8">
         <v>1</v>
@@ -2230,16 +2239,16 @@
         <f> B27+C27</f>
       </c>
       <c r="E27" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -2248,7 +2257,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B28" s="8">
         <v>1</v>
@@ -2260,16 +2269,16 @@
         <f> B28+C28</f>
       </c>
       <c r="E28" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -2278,7 +2287,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B29" s="8">
         <v>1</v>
@@ -2290,16 +2299,16 @@
         <f> B29+C29</f>
       </c>
       <c r="E29" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -2308,7 +2317,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B30" s="8">
         <v>1</v>
@@ -2320,16 +2329,16 @@
         <f> B30+C30</f>
       </c>
       <c r="E30" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -2338,7 +2347,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B31" s="8">
         <v>1</v>
@@ -2350,16 +2359,16 @@
         <f> B31+C31</f>
       </c>
       <c r="E31" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -2368,7 +2377,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B32" s="8">
         <v>1</v>
@@ -2380,16 +2389,16 @@
         <f> B32+C32</f>
       </c>
       <c r="E32" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -2585,10 +2594,10 @@
         <f>Farmers!D5</f>
       </c>
       <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="G5" s="8">
         <v>135</v>
@@ -2609,17 +2618,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="13">
         <f>Farmers!D6</f>
       </c>
       <c r="E6" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>28</v>
@@ -2723,10 +2732,10 @@
         <f>Farmers!D9</f>
       </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G9" s="8">
         <v>125</v>
@@ -2745,25 +2754,25 @@
         <v>2</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="7">
         <f>Farmers!D10</f>
       </c>
       <c r="E10" s="4" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>28</v>
@@ -2782,7 +2791,7 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M10" s="22">
         <v>126.1</v>
@@ -2793,17 +2802,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="13">
         <f>Farmers!D11</f>
       </c>
       <c r="E11" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>28</v>
@@ -2822,7 +2831,7 @@
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M11" s="23">
         <v>126.12</v>
@@ -2833,22 +2842,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12" s="18">
         <f>Farmers!D12</f>
       </c>
       <c r="E12" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G12" s="19">
         <v>115</v>
@@ -2864,7 +2873,7 @@
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M12" s="23">
         <v>120.6</v>
@@ -2875,20 +2884,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="7">
         <f>Farmers!D13</f>
       </c>
       <c r="E13" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="G13" s="8">
         <v>125</v>
@@ -2904,7 +2913,7 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M13" s="24">
         <v>119.3</v>
@@ -2915,20 +2924,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="7">
         <f>Farmers!D14</f>
       </c>
       <c r="E14" s="4" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G14" s="8">
         <v>123</v>
@@ -2949,20 +2958,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="7">
         <f>Farmers!D15</f>
       </c>
       <c r="E15" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G15" s="8">
         <v>115</v>
@@ -2983,20 +2992,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13">
         <f>Farmers!D16</f>
       </c>
       <c r="E16" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G16" s="14">
         <v>125</v>
@@ -3017,22 +3026,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D17" s="18">
         <f>Farmers!D17</f>
       </c>
       <c r="E17" s="16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="G17" s="19">
         <v>110</v>
@@ -3053,20 +3062,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="7">
         <f>Farmers!D18</f>
       </c>
       <c r="E18" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G18" s="8">
         <v>120</v>
@@ -3087,20 +3096,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="7">
         <f>Farmers!D19</f>
       </c>
       <c r="E19" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G19" s="8">
         <v>105</v>
@@ -3121,20 +3130,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="7">
         <f>Farmers!D20</f>
       </c>
       <c r="E20" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G20" s="8">
         <v>130</v>
@@ -3155,20 +3164,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="13">
         <f>Farmers!D21</f>
       </c>
       <c r="E21" s="11" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G21" s="14">
         <v>130</v>

</xml_diff>